<commit_message>
fixed ryi booking process issue.
</commit_message>
<xml_diff>
--- a/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
+++ b/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\HD\MY20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\bitbucket\hd-emea-test-script\proj12_ryi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="313">
   <si>
     <t>Region</t>
   </si>
@@ -1006,6 +1006,9 @@
   </si>
   <si>
     <t>FXLR</t>
+  </si>
+  <si>
+    <t>FXDRS</t>
   </si>
 </sst>
 </file>
@@ -2009,10 +2012,10 @@
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y8" sqref="Y8"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2070,7 +2073,7 @@
         <v>309</v>
       </c>
       <c r="R1" s="24" t="s">
-        <v>69</v>
+        <v>312</v>
       </c>
       <c r="S1" s="24" t="s">
         <v>310</v>

</xml_diff>

<commit_message>
fixed bike list check issue.
</commit_message>
<xml_diff>
--- a/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
+++ b/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="314">
   <si>
     <t>Region</t>
   </si>
@@ -1009,6 +1009,9 @@
   </si>
   <si>
     <t>FXDRS</t>
+  </si>
+  <si>
+    <t>FLHC</t>
   </si>
 </sst>
 </file>
@@ -2015,7 +2018,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2079,7 +2082,7 @@
         <v>310</v>
       </c>
       <c r="T1" s="24" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="U1" s="24" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Add tracking code checking.
</commit_message>
<xml_diff>
--- a/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
+++ b/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
@@ -1011,7 +1011,7 @@
     <t>FLHC</t>
   </si>
   <si>
-    <t>FXBRS</t>
+    <t>FXBR</t>
   </si>
 </sst>
 </file>
@@ -2018,7 +2018,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
update matrix bikedid and matrix utils.
</commit_message>
<xml_diff>
--- a/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
+++ b/proj12_ryi/data/MY20-RYI-Matrix-V4.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="316">
   <si>
     <t>Region</t>
   </si>
@@ -1012,6 +1012,12 @@
   </si>
   <si>
     <t>FXBR</t>
+  </si>
+  <si>
+    <t>Breakout 114</t>
+  </si>
+  <si>
+    <t>FXBRS</t>
   </si>
 </sst>
 </file>
@@ -2012,13 +2018,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y49"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2037,19 +2043,19 @@
     <col min="12" max="12" width="19.625" style="5" customWidth="1"/>
     <col min="13" max="14" width="18.5" style="5" customWidth="1"/>
     <col min="15" max="15" width="19.625" style="5" customWidth="1"/>
-    <col min="16" max="17" width="18.5" style="5" customWidth="1"/>
-    <col min="18" max="18" width="19.875" style="5" customWidth="1"/>
-    <col min="19" max="19" width="18.5" style="5" customWidth="1"/>
-    <col min="20" max="20" width="19.625" style="5" customWidth="1"/>
-    <col min="21" max="21" width="18.5" style="5" customWidth="1"/>
-    <col min="22" max="22" width="57.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="65" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="50.375" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="63.125" style="12" customWidth="1"/>
-    <col min="26" max="16384" width="11.125" style="5"/>
+    <col min="16" max="18" width="18.5" style="5" customWidth="1"/>
+    <col min="19" max="19" width="19.875" style="5" customWidth="1"/>
+    <col min="20" max="20" width="18.5" style="5" customWidth="1"/>
+    <col min="21" max="21" width="19.625" style="5" customWidth="1"/>
+    <col min="22" max="22" width="18.5" style="5" customWidth="1"/>
+    <col min="23" max="23" width="57.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="65" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="50.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="63.125" style="12" customWidth="1"/>
+    <col min="27" max="16384" width="11.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="10" t="s">
         <v>266</v>
       </c>
@@ -2076,20 +2082,23 @@
         <v>313</v>
       </c>
       <c r="R1" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="S1" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="S1" s="24" t="s">
+      <c r="T1" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="U1" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="V1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="24"/>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="24"/>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="10" t="s">
         <v>267</v>
       </c>
@@ -2103,15 +2112,16 @@
       <c r="P2" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="Q2" s="90"/>
+      <c r="Q2" s="91"/>
       <c r="R2" s="90"/>
-      <c r="S2" s="92" t="s">
+      <c r="S2" s="90"/>
+      <c r="T2" s="92" t="s">
         <v>270</v>
       </c>
-      <c r="T2" s="90"/>
       <c r="U2" s="90"/>
-    </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" ht="16.5" thickBot="1">
+      <c r="V2" s="90"/>
+    </row>
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="16.5" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2164,31 +2174,34 @@
         <v>68</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="U3" s="26" t="s">
+      <c r="V3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="V3" s="57" t="s">
+      <c r="W3" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="W3" s="57" t="s">
+      <c r="X3" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="X3" s="57" t="s">
+      <c r="Y3" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="Y3" s="27" t="s">
+      <c r="Z3" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:26">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -2240,8 +2253,8 @@
       <c r="Q4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="17" t="s">
-        <v>10</v>
+      <c r="R4" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S4" s="17" t="s">
         <v>10</v>
@@ -2252,18 +2265,21 @@
       <c r="U4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="58" t="s">
+      <c r="V4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="W4" s="58" t="s">
+      <c r="X4" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="X4" s="58" t="s">
+      <c r="Y4" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="Y4" s="13"/>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="Z4" s="13"/>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -2315,8 +2331,8 @@
       <c r="Q5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="17" t="s">
-        <v>10</v>
+      <c r="R5" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S5" s="17" t="s">
         <v>10</v>
@@ -2324,21 +2340,24 @@
       <c r="T5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V5" s="58" t="s">
+      <c r="U5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="W5" s="58" t="s">
+      <c r="X5" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="X5" s="58" t="s">
+      <c r="Y5" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="Y5" s="15"/>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="Z5" s="15"/>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -2387,8 +2406,8 @@
       <c r="P6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>10</v>
+      <c r="Q6" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="R6" s="17" t="s">
         <v>10</v>
@@ -2399,21 +2418,24 @@
       <c r="T6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V6" s="58" t="s">
+      <c r="U6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="W6" s="58" t="s">
+      <c r="X6" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="X6" s="58" t="s">
+      <c r="Y6" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="Y6" s="14"/>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="Z6" s="14"/>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -2462,8 +2484,8 @@
       <c r="P7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="17" t="s">
-        <v>10</v>
+      <c r="Q7" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="R7" s="17" t="s">
         <v>10</v>
@@ -2474,21 +2496,24 @@
       <c r="T7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V7" s="59" t="s">
+      <c r="U7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="W7" s="60" t="s">
+      <c r="X7" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="X7" s="60" t="s">
+      <c r="Y7" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="Y7" s="14"/>
-    </row>
-    <row r="8" spans="1:25" ht="16.5" thickBot="1">
+      <c r="Z7" s="14"/>
+    </row>
+    <row r="8" spans="1:26" ht="16.5" thickBot="1">
       <c r="A8" s="18" t="s">
         <v>8</v>
       </c>
@@ -2540,8 +2565,8 @@
       <c r="Q8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="21" t="s">
-        <v>10</v>
+      <c r="R8" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S8" s="21" t="s">
         <v>10</v>
@@ -2552,16 +2577,19 @@
       <c r="U8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="58" t="s">
+      <c r="V8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="W8" s="58" t="s">
+      <c r="X8" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="X8" s="61"/>
-      <c r="Y8" s="15"/>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="Y8" s="61"/>
+      <c r="Z8" s="15"/>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -2613,8 +2641,8 @@
       <c r="Q9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R9" s="17" t="s">
-        <v>10</v>
+      <c r="R9" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S9" s="17" t="s">
         <v>10</v>
@@ -2625,16 +2653,19 @@
       <c r="U9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="V9" s="59" t="s">
+      <c r="V9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="W9" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="W9" s="62" t="s">
+      <c r="X9" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="X9" s="63"/>
-      <c r="Y9" s="15"/>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="Y9" s="63"/>
+      <c r="Z9" s="15"/>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
@@ -2686,8 +2717,8 @@
       <c r="Q10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R10" s="17" t="s">
-        <v>10</v>
+      <c r="R10" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S10" s="17" t="s">
         <v>10</v>
@@ -2695,19 +2726,22 @@
       <c r="T10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V10" s="58" t="s">
+      <c r="U10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W10" s="58" t="s">
+      <c r="X10" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="X10" s="63"/>
-      <c r="Y10" s="15"/>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="Y10" s="63"/>
+      <c r="Z10" s="15"/>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
@@ -2759,8 +2793,8 @@
       <c r="Q11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R11" s="17" t="s">
-        <v>10</v>
+      <c r="R11" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S11" s="17" t="s">
         <v>10</v>
@@ -2768,19 +2802,22 @@
       <c r="T11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V11" s="58" t="s">
+      <c r="U11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="W11" s="58" t="s">
+      <c r="X11" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="X11" s="63"/>
-      <c r="Y11" s="15"/>
-    </row>
-    <row r="12" spans="1:25" s="8" customFormat="1">
+      <c r="Y11" s="63"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" spans="1:26" s="8" customFormat="1">
       <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
@@ -2832,8 +2869,8 @@
       <c r="Q12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R12" s="17" t="s">
-        <v>10</v>
+      <c r="R12" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S12" s="17" t="s">
         <v>10</v>
@@ -2841,19 +2878,22 @@
       <c r="T12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V12" s="58" t="s">
+      <c r="U12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="W12" s="58" t="s">
+      <c r="X12" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="14"/>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="Y12" s="63"/>
+      <c r="Z12" s="14"/>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -2905,8 +2945,8 @@
       <c r="Q13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R13" s="17" t="s">
-        <v>10</v>
+      <c r="R13" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S13" s="17" t="s">
         <v>10</v>
@@ -2914,19 +2954,22 @@
       <c r="T13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V13" s="58" t="s">
+      <c r="U13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W13" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="W13" s="58" t="s">
+      <c r="X13" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="X13" s="63"/>
-      <c r="Y13" s="14"/>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="Y13" s="63"/>
+      <c r="Z13" s="14"/>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
@@ -2978,8 +3021,8 @@
       <c r="Q14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R14" s="17" t="s">
-        <v>10</v>
+      <c r="R14" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>10</v>
@@ -2987,21 +3030,24 @@
       <c r="T14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V14" s="58" t="s">
+      <c r="U14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="W14" s="58" t="s">
+      <c r="X14" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="X14" s="58" t="s">
+      <c r="Y14" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="Y14" s="14"/>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="Z14" s="14"/>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -3053,8 +3099,8 @@
       <c r="Q15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R15" s="17" t="s">
-        <v>10</v>
+      <c r="R15" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S15" s="17" t="s">
         <v>10</v>
@@ -3062,17 +3108,20 @@
       <c r="T15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V15" s="60" t="s">
+      <c r="U15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W15" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="W15" s="63"/>
       <c r="X15" s="63"/>
-      <c r="Y15" s="14"/>
-    </row>
-    <row r="16" spans="1:25" s="8" customFormat="1">
+      <c r="Y15" s="63"/>
+      <c r="Z15" s="14"/>
+    </row>
+    <row r="16" spans="1:26" s="8" customFormat="1">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -3124,8 +3173,8 @@
       <c r="Q16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R16" s="17" t="s">
-        <v>10</v>
+      <c r="R16" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S16" s="17" t="s">
         <v>10</v>
@@ -3133,19 +3182,22 @@
       <c r="T16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V16" s="58" t="s">
+      <c r="U16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W16" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W16" s="58" t="s">
+      <c r="X16" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X16" s="63"/>
-      <c r="Y16" s="14"/>
-    </row>
-    <row r="17" spans="1:25">
+      <c r="Y16" s="63"/>
+      <c r="Z16" s="14"/>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
@@ -3197,8 +3249,8 @@
       <c r="Q17" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R17" s="17" t="s">
-        <v>10</v>
+      <c r="R17" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S17" s="17" t="s">
         <v>10</v>
@@ -3206,19 +3258,22 @@
       <c r="T17" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V17" s="58" t="s">
+      <c r="U17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W17" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W17" s="58" t="s">
+      <c r="X17" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X17" s="63"/>
-      <c r="Y17" s="14"/>
-    </row>
-    <row r="18" spans="1:25">
+      <c r="Y17" s="63"/>
+      <c r="Z17" s="14"/>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -3270,8 +3325,8 @@
       <c r="Q18" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R18" s="17" t="s">
-        <v>10</v>
+      <c r="R18" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S18" s="17" t="s">
         <v>10</v>
@@ -3279,21 +3334,24 @@
       <c r="T18" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V18" s="63" t="s">
+      <c r="U18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W18" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="W18" s="63" t="s">
+      <c r="X18" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="X18" s="63" t="s">
+      <c r="Y18" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="Y18" s="14"/>
-    </row>
-    <row r="19" spans="1:25">
+      <c r="Z18" s="14"/>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
@@ -3345,8 +3403,8 @@
       <c r="Q19" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R19" s="17" t="s">
-        <v>10</v>
+      <c r="R19" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S19" s="17" t="s">
         <v>10</v>
@@ -3354,21 +3412,24 @@
       <c r="T19" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V19" s="58" t="s">
+      <c r="U19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W19" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="W19" s="58" t="s">
+      <c r="X19" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="X19" s="58" t="s">
+      <c r="Y19" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="Y19" s="14"/>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="Z19" s="14"/>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -3420,8 +3481,8 @@
       <c r="Q20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R20" s="17" t="s">
-        <v>10</v>
+      <c r="R20" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S20" s="17" t="s">
         <v>10</v>
@@ -3429,17 +3490,20 @@
       <c r="T20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V20" s="58" t="s">
+      <c r="U20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W20" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="W20" s="58"/>
-      <c r="X20" s="63"/>
-      <c r="Y20" s="14"/>
-    </row>
-    <row r="21" spans="1:25" ht="17.100000000000001" customHeight="1">
+      <c r="X20" s="58"/>
+      <c r="Y20" s="63"/>
+      <c r="Z20" s="14"/>
+    </row>
+    <row r="21" spans="1:26" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
@@ -3491,8 +3555,8 @@
       <c r="Q21" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R21" s="17" t="s">
-        <v>10</v>
+      <c r="R21" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S21" s="17" t="s">
         <v>10</v>
@@ -3500,21 +3564,24 @@
       <c r="T21" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V21" s="58" t="s">
+      <c r="U21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W21" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="W21" s="58" t="s">
+      <c r="X21" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="X21" s="58" t="s">
+      <c r="Y21" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="Y21" s="14"/>
-    </row>
-    <row r="22" spans="1:25">
+      <c r="Z21" s="14"/>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
@@ -3566,8 +3633,8 @@
       <c r="Q22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R22" s="17" t="s">
-        <v>10</v>
+      <c r="R22" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S22" s="17" t="s">
         <v>10</v>
@@ -3575,19 +3642,22 @@
       <c r="T22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V22" s="58" t="s">
+      <c r="U22" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W22" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="W22" s="58" t="s">
+      <c r="X22" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="X22" s="63"/>
-      <c r="Y22" s="14"/>
-    </row>
-    <row r="23" spans="1:25">
+      <c r="Y22" s="63"/>
+      <c r="Z22" s="14"/>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23" s="6" t="s">
         <v>26</v>
       </c>
@@ -3639,8 +3709,8 @@
       <c r="Q23" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R23" s="17" t="s">
-        <v>10</v>
+      <c r="R23" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S23" s="17" t="s">
         <v>10</v>
@@ -3648,21 +3718,24 @@
       <c r="T23" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U23" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V23" s="58" t="s">
+      <c r="U23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W23" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="W23" s="58" t="s">
+      <c r="X23" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="X23" s="58" t="s">
+      <c r="Y23" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="Y23" s="14"/>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="Z23" s="14"/>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
@@ -3714,8 +3787,8 @@
       <c r="Q24" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R24" s="17" t="s">
-        <v>10</v>
+      <c r="R24" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S24" s="17" t="s">
         <v>10</v>
@@ -3723,21 +3796,24 @@
       <c r="T24" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U24" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V24" s="58" t="s">
+      <c r="U24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W24" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="W24" s="58" t="s">
+      <c r="X24" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="X24" s="58" t="s">
+      <c r="Y24" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="Y24" s="14"/>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="Z24" s="14"/>
+    </row>
+    <row r="25" spans="1:26">
       <c r="A25" s="6" t="s">
         <v>26</v>
       </c>
@@ -3789,8 +3865,8 @@
       <c r="Q25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R25" s="17" t="s">
-        <v>10</v>
+      <c r="R25" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S25" s="17" t="s">
         <v>10</v>
@@ -3798,17 +3874,20 @@
       <c r="T25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V25" s="59" t="s">
+      <c r="U25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W25" s="59" t="s">
         <v>173</v>
       </c>
-      <c r="W25" s="63"/>
       <c r="X25" s="63"/>
-      <c r="Y25" s="14"/>
-    </row>
-    <row r="26" spans="1:25">
+      <c r="Y25" s="63"/>
+      <c r="Z25" s="14"/>
+    </row>
+    <row r="26" spans="1:26">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -3860,8 +3939,8 @@
       <c r="Q26" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R26" s="17" t="s">
-        <v>10</v>
+      <c r="R26" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S26" s="17" t="s">
         <v>10</v>
@@ -3869,19 +3948,22 @@
       <c r="T26" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V26" s="58" t="s">
+      <c r="U26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W26" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="W26" s="58" t="s">
+      <c r="X26" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="X26" s="63"/>
-      <c r="Y26" s="14"/>
-    </row>
-    <row r="27" spans="1:25" s="8" customFormat="1">
+      <c r="Y26" s="63"/>
+      <c r="Z26" s="14"/>
+    </row>
+    <row r="27" spans="1:26" s="8" customFormat="1">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -3933,8 +4015,8 @@
       <c r="Q27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R27" s="17" t="s">
-        <v>10</v>
+      <c r="R27" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S27" s="17" t="s">
         <v>10</v>
@@ -3942,21 +4024,24 @@
       <c r="T27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U27" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V27" s="58" t="s">
+      <c r="U27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W27" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="W27" s="58" t="s">
+      <c r="X27" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="X27" s="58" t="s">
+      <c r="Y27" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="Y27" s="16"/>
-    </row>
-    <row r="28" spans="1:25" s="8" customFormat="1">
+      <c r="Z27" s="16"/>
+    </row>
+    <row r="28" spans="1:26" s="8" customFormat="1">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
@@ -4008,8 +4093,8 @@
       <c r="Q28" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R28" s="17" t="s">
-        <v>10</v>
+      <c r="R28" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S28" s="17" t="s">
         <v>10</v>
@@ -4017,21 +4102,24 @@
       <c r="T28" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U28" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V28" s="58" t="s">
+      <c r="U28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W28" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="W28" s="58" t="s">
+      <c r="X28" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="X28" s="58" t="s">
+      <c r="Y28" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="Y28" s="14"/>
-    </row>
-    <row r="29" spans="1:25" s="8" customFormat="1">
+      <c r="Z28" s="14"/>
+    </row>
+    <row r="29" spans="1:26" s="8" customFormat="1">
       <c r="A29" s="6" t="s">
         <v>26</v>
       </c>
@@ -4083,8 +4171,8 @@
       <c r="Q29" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R29" s="17" t="s">
-        <v>10</v>
+      <c r="R29" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S29" s="17" t="s">
         <v>10</v>
@@ -4092,21 +4180,24 @@
       <c r="T29" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V29" s="58" t="s">
+      <c r="U29" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W29" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="W29" s="58" t="s">
+      <c r="X29" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="X29" s="58" t="s">
+      <c r="Y29" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="Y29" s="14"/>
-    </row>
-    <row r="30" spans="1:25">
+      <c r="Z29" s="14"/>
+    </row>
+    <row r="30" spans="1:26">
       <c r="A30" s="6" t="s">
         <v>26</v>
       </c>
@@ -4158,8 +4249,8 @@
       <c r="Q30" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R30" s="17" t="s">
-        <v>10</v>
+      <c r="R30" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S30" s="17" t="s">
         <v>10</v>
@@ -4167,21 +4258,24 @@
       <c r="T30" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V30" s="58" t="s">
+      <c r="U30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W30" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="W30" s="58" t="s">
+      <c r="X30" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="X30" s="58" t="s">
+      <c r="Y30" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="Y30" s="14"/>
-    </row>
-    <row r="31" spans="1:25">
+      <c r="Z30" s="14"/>
+    </row>
+    <row r="31" spans="1:26">
       <c r="A31" s="6" t="s">
         <v>26</v>
       </c>
@@ -4233,8 +4327,8 @@
       <c r="Q31" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R31" s="17" t="s">
-        <v>10</v>
+      <c r="R31" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S31" s="17" t="s">
         <v>10</v>
@@ -4242,19 +4336,22 @@
       <c r="T31" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U31" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V31" s="59" t="s">
+      <c r="U31" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W31" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="W31" s="62" t="s">
+      <c r="X31" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="X31" s="63"/>
-      <c r="Y31" s="14"/>
-    </row>
-    <row r="32" spans="1:25">
+      <c r="Y31" s="63"/>
+      <c r="Z31" s="14"/>
+    </row>
+    <row r="32" spans="1:26">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4306,8 +4403,8 @@
       <c r="Q32" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R32" s="17" t="s">
-        <v>10</v>
+      <c r="R32" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S32" s="17" t="s">
         <v>10</v>
@@ -4315,21 +4412,24 @@
       <c r="T32" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U32" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V32" s="58" t="s">
+      <c r="U32" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W32" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="W32" s="58" t="s">
+      <c r="X32" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="X32" s="58" t="s">
+      <c r="Y32" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="Y32" s="14"/>
-    </row>
-    <row r="33" spans="1:25" s="8" customFormat="1">
+      <c r="Z32" s="14"/>
+    </row>
+    <row r="33" spans="1:26" s="8" customFormat="1">
       <c r="A33" s="6" t="s">
         <v>26</v>
       </c>
@@ -4381,8 +4481,8 @@
       <c r="Q33" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R33" s="17" t="s">
-        <v>10</v>
+      <c r="R33" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S33" s="17" t="s">
         <v>10</v>
@@ -4390,19 +4490,22 @@
       <c r="T33" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U33" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V33" s="58" t="s">
+      <c r="U33" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W33" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="W33" s="58" t="s">
+      <c r="X33" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="X33" s="63"/>
-      <c r="Y33" s="14"/>
-    </row>
-    <row r="34" spans="1:25">
+      <c r="Y33" s="63"/>
+      <c r="Z33" s="14"/>
+    </row>
+    <row r="34" spans="1:26">
       <c r="A34" s="6" t="s">
         <v>26</v>
       </c>
@@ -4454,8 +4557,8 @@
       <c r="Q34" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R34" s="17" t="s">
-        <v>10</v>
+      <c r="R34" s="79" t="s">
+        <v>291</v>
       </c>
       <c r="S34" s="17" t="s">
         <v>10</v>
@@ -4463,17 +4566,20 @@
       <c r="T34" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U34" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V34" s="58" t="s">
+      <c r="U34" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="V34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W34" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="W34" s="58"/>
       <c r="X34" s="58"/>
-      <c r="Y34" s="14"/>
-    </row>
-    <row r="35" spans="1:25">
+      <c r="Y34" s="58"/>
+      <c r="Z34" s="14"/>
+    </row>
+    <row r="35" spans="1:26">
       <c r="A35" s="28" t="s">
         <v>16</v>
       </c>
@@ -4529,16 +4635,19 @@
         <v>11</v>
       </c>
       <c r="U35" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="V35" s="31"/>
+        <v>11</v>
+      </c>
+      <c r="V35" s="30" t="s">
+        <v>10</v>
+      </c>
       <c r="W35" s="31"/>
       <c r="X35" s="31"/>
-      <c r="Y35" s="32" t="s">
+      <c r="Y35" s="31"/>
+      <c r="Z35" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:26">
       <c r="A36" s="33" t="s">
         <v>16</v>
       </c>
@@ -4593,17 +4702,20 @@
       <c r="T36" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U36" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V36" s="36"/>
+      <c r="U36" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V36" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W36" s="36"/>
       <c r="X36" s="36"/>
-      <c r="Y36" s="32" t="s">
+      <c r="Y36" s="36"/>
+      <c r="Z36" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:26">
       <c r="A37" s="33" t="s">
         <v>16</v>
       </c>
@@ -4658,17 +4770,20 @@
       <c r="T37" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U37" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V37" s="36"/>
+      <c r="U37" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V37" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W37" s="36"/>
       <c r="X37" s="36"/>
-      <c r="Y37" s="32" t="s">
+      <c r="Y37" s="36"/>
+      <c r="Z37" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:26">
       <c r="A38" s="33" t="s">
         <v>16</v>
       </c>
@@ -4723,17 +4838,20 @@
       <c r="T38" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U38" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V38" s="36"/>
+      <c r="U38" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V38" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W38" s="36"/>
       <c r="X38" s="36"/>
-      <c r="Y38" s="32" t="s">
+      <c r="Y38" s="36"/>
+      <c r="Z38" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:26">
       <c r="A39" s="33" t="s">
         <v>16</v>
       </c>
@@ -4788,17 +4906,20 @@
       <c r="T39" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U39" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V39" s="36"/>
+      <c r="U39" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V39" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W39" s="36"/>
       <c r="X39" s="36"/>
-      <c r="Y39" s="32" t="s">
+      <c r="Y39" s="36"/>
+      <c r="Z39" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:26">
       <c r="A40" s="33" t="s">
         <v>16</v>
       </c>
@@ -4853,17 +4974,20 @@
       <c r="T40" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U40" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V40" s="36"/>
+      <c r="U40" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V40" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W40" s="36"/>
       <c r="X40" s="36"/>
-      <c r="Y40" s="32" t="s">
+      <c r="Y40" s="36"/>
+      <c r="Z40" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:26">
       <c r="A41" s="33" t="s">
         <v>16</v>
       </c>
@@ -4918,17 +5042,20 @@
       <c r="T41" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U41" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V41" s="36"/>
+      <c r="U41" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V41" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W41" s="36"/>
       <c r="X41" s="36"/>
-      <c r="Y41" s="32" t="s">
+      <c r="Y41" s="36"/>
+      <c r="Z41" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:26">
       <c r="A42" s="33" t="s">
         <v>16</v>
       </c>
@@ -4983,17 +5110,20 @@
       <c r="T42" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U42" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V42" s="36"/>
+      <c r="U42" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V42" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W42" s="36"/>
       <c r="X42" s="36"/>
-      <c r="Y42" s="32" t="s">
+      <c r="Y42" s="36"/>
+      <c r="Z42" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:25" s="8" customFormat="1">
+    <row r="43" spans="1:26" s="8" customFormat="1">
       <c r="A43" s="33" t="s">
         <v>16</v>
       </c>
@@ -5048,17 +5178,20 @@
       <c r="T43" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U43" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="V43" s="36"/>
+      <c r="U43" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="V43" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W43" s="36"/>
       <c r="X43" s="36"/>
-      <c r="Y43" s="32" t="s">
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="16.5" thickBot="1">
+    <row r="44" spans="1:26" ht="16.5" thickBot="1">
       <c r="A44" s="37" t="s">
         <v>16</v>
       </c>
@@ -5114,25 +5247,28 @@
         <v>11</v>
       </c>
       <c r="U44" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="V44" s="40"/>
+        <v>11</v>
+      </c>
+      <c r="V44" s="39" t="s">
+        <v>10</v>
+      </c>
       <c r="W44" s="40"/>
       <c r="X44" s="40"/>
-      <c r="Y44" s="41" t="s">
+      <c r="Y44" s="40"/>
+      <c r="Z44" s="41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="18.75">
+    <row r="46" spans="1:26" ht="18.75">
       <c r="B46" s="84" t="s">
         <v>295</v>
       </c>
-      <c r="V46" s="5"/>
       <c r="W46" s="5"/>
       <c r="X46" s="5"/>
       <c r="Y46" s="5"/>
-    </row>
-    <row r="47" spans="1:25" s="8" customFormat="1">
+      <c r="Z46" s="5"/>
+    </row>
+    <row r="47" spans="1:26" s="8" customFormat="1">
       <c r="A47" s="6" t="s">
         <v>26</v>
       </c>
@@ -5140,113 +5276,113 @@
         <v>296</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:26">
       <c r="A48" s="88" t="s">
         <v>26</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="V48" s="5"/>
       <c r="W48" s="5"/>
       <c r="X48" s="5"/>
       <c r="Y48" s="5"/>
-    </row>
-    <row r="49" spans="1:25">
+      <c r="Z48" s="5"/>
+    </row>
+    <row r="49" spans="1:26">
       <c r="A49" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="V49" s="5"/>
       <c r="W49" s="5"/>
       <c r="X49" s="5"/>
       <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:V2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="V9">
+  <conditionalFormatting sqref="W9">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V31">
+  <conditionalFormatting sqref="W31">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2" display="http://h-d.com/ridefree"/>
-    <hyperlink ref="V8" r:id="rId3"/>
-    <hyperlink ref="V7" r:id="rId4"/>
-    <hyperlink ref="V6" r:id="rId5"/>
-    <hyperlink ref="V16" r:id="rId6"/>
-    <hyperlink ref="V17" r:id="rId7"/>
-    <hyperlink ref="V23" r:id="rId8"/>
-    <hyperlink ref="V14" r:id="rId9"/>
-    <hyperlink ref="V19" r:id="rId10"/>
-    <hyperlink ref="V32" r:id="rId11"/>
-    <hyperlink ref="V27" r:id="rId12"/>
-    <hyperlink ref="V4" r:id="rId13"/>
-    <hyperlink ref="V5" r:id="rId14"/>
-    <hyperlink ref="V11" r:id="rId15"/>
-    <hyperlink ref="V13" r:id="rId16"/>
-    <hyperlink ref="V22" r:id="rId17"/>
-    <hyperlink ref="V26" r:id="rId18"/>
-    <hyperlink ref="V12" r:id="rId19"/>
-    <hyperlink ref="V21" r:id="rId20"/>
-    <hyperlink ref="V28" r:id="rId21"/>
-    <hyperlink ref="V24" r:id="rId22"/>
-    <hyperlink ref="V29" r:id="rId23"/>
-    <hyperlink ref="V25" r:id="rId24"/>
-    <hyperlink ref="V9" r:id="rId25"/>
-    <hyperlink ref="V31" r:id="rId26"/>
-    <hyperlink ref="V33" r:id="rId27"/>
-    <hyperlink ref="W8" r:id="rId28"/>
-    <hyperlink ref="W6" r:id="rId29"/>
-    <hyperlink ref="W16" r:id="rId30"/>
-    <hyperlink ref="W17" r:id="rId31"/>
-    <hyperlink ref="W23" r:id="rId32"/>
-    <hyperlink ref="W14" r:id="rId33"/>
-    <hyperlink ref="W19" r:id="rId34"/>
-    <hyperlink ref="W32" r:id="rId35"/>
-    <hyperlink ref="W27" r:id="rId36"/>
-    <hyperlink ref="W4" r:id="rId37"/>
-    <hyperlink ref="W5" r:id="rId38"/>
-    <hyperlink ref="W11" r:id="rId39"/>
-    <hyperlink ref="W13" r:id="rId40"/>
-    <hyperlink ref="W22" r:id="rId41"/>
-    <hyperlink ref="W26" r:id="rId42"/>
-    <hyperlink ref="W12" r:id="rId43"/>
-    <hyperlink ref="W21" r:id="rId44"/>
-    <hyperlink ref="W28" r:id="rId45"/>
-    <hyperlink ref="W24" r:id="rId46"/>
-    <hyperlink ref="W29" r:id="rId47"/>
-    <hyperlink ref="W33" r:id="rId48"/>
-    <hyperlink ref="X6" r:id="rId49"/>
-    <hyperlink ref="X14" r:id="rId50"/>
-    <hyperlink ref="X23" r:id="rId51"/>
-    <hyperlink ref="X19" r:id="rId52"/>
-    <hyperlink ref="X32" r:id="rId53"/>
-    <hyperlink ref="X27" r:id="rId54"/>
-    <hyperlink ref="X4" r:id="rId55"/>
-    <hyperlink ref="X5" r:id="rId56"/>
-    <hyperlink ref="X21" r:id="rId57"/>
-    <hyperlink ref="X28" r:id="rId58"/>
-    <hyperlink ref="X24" r:id="rId59"/>
-    <hyperlink ref="X29" r:id="rId60"/>
-    <hyperlink ref="W9" r:id="rId61"/>
-    <hyperlink ref="W31" r:id="rId62"/>
-    <hyperlink ref="V34" r:id="rId63"/>
-    <hyperlink ref="X30" r:id="rId64"/>
-    <hyperlink ref="V30" r:id="rId65"/>
-    <hyperlink ref="W30" r:id="rId66"/>
-    <hyperlink ref="V20" r:id="rId67"/>
-    <hyperlink ref="V10" r:id="rId68"/>
-    <hyperlink ref="W10" r:id="rId69"/>
+    <hyperlink ref="W8" r:id="rId3"/>
+    <hyperlink ref="W7" r:id="rId4"/>
+    <hyperlink ref="W6" r:id="rId5"/>
+    <hyperlink ref="W16" r:id="rId6"/>
+    <hyperlink ref="W17" r:id="rId7"/>
+    <hyperlink ref="W23" r:id="rId8"/>
+    <hyperlink ref="W14" r:id="rId9"/>
+    <hyperlink ref="W19" r:id="rId10"/>
+    <hyperlink ref="W32" r:id="rId11"/>
+    <hyperlink ref="W27" r:id="rId12"/>
+    <hyperlink ref="W4" r:id="rId13"/>
+    <hyperlink ref="W5" r:id="rId14"/>
+    <hyperlink ref="W11" r:id="rId15"/>
+    <hyperlink ref="W13" r:id="rId16"/>
+    <hyperlink ref="W22" r:id="rId17"/>
+    <hyperlink ref="W26" r:id="rId18"/>
+    <hyperlink ref="W12" r:id="rId19"/>
+    <hyperlink ref="W21" r:id="rId20"/>
+    <hyperlink ref="W28" r:id="rId21"/>
+    <hyperlink ref="W24" r:id="rId22"/>
+    <hyperlink ref="W29" r:id="rId23"/>
+    <hyperlink ref="W25" r:id="rId24"/>
+    <hyperlink ref="W9" r:id="rId25"/>
+    <hyperlink ref="W31" r:id="rId26"/>
+    <hyperlink ref="W33" r:id="rId27"/>
+    <hyperlink ref="X8" r:id="rId28"/>
+    <hyperlink ref="X6" r:id="rId29"/>
+    <hyperlink ref="X16" r:id="rId30"/>
+    <hyperlink ref="X17" r:id="rId31"/>
+    <hyperlink ref="X23" r:id="rId32"/>
+    <hyperlink ref="X14" r:id="rId33"/>
+    <hyperlink ref="X19" r:id="rId34"/>
+    <hyperlink ref="X32" r:id="rId35"/>
+    <hyperlink ref="X27" r:id="rId36"/>
+    <hyperlink ref="X4" r:id="rId37"/>
+    <hyperlink ref="X5" r:id="rId38"/>
+    <hyperlink ref="X11" r:id="rId39"/>
+    <hyperlink ref="X13" r:id="rId40"/>
+    <hyperlink ref="X22" r:id="rId41"/>
+    <hyperlink ref="X26" r:id="rId42"/>
+    <hyperlink ref="X12" r:id="rId43"/>
+    <hyperlink ref="X21" r:id="rId44"/>
+    <hyperlink ref="X28" r:id="rId45"/>
+    <hyperlink ref="X24" r:id="rId46"/>
+    <hyperlink ref="X29" r:id="rId47"/>
+    <hyperlink ref="X33" r:id="rId48"/>
+    <hyperlink ref="Y6" r:id="rId49"/>
+    <hyperlink ref="Y14" r:id="rId50"/>
+    <hyperlink ref="Y23" r:id="rId51"/>
+    <hyperlink ref="Y19" r:id="rId52"/>
+    <hyperlink ref="Y32" r:id="rId53"/>
+    <hyperlink ref="Y27" r:id="rId54"/>
+    <hyperlink ref="Y4" r:id="rId55"/>
+    <hyperlink ref="Y5" r:id="rId56"/>
+    <hyperlink ref="Y21" r:id="rId57"/>
+    <hyperlink ref="Y28" r:id="rId58"/>
+    <hyperlink ref="Y24" r:id="rId59"/>
+    <hyperlink ref="Y29" r:id="rId60"/>
+    <hyperlink ref="X9" r:id="rId61"/>
+    <hyperlink ref="X31" r:id="rId62"/>
+    <hyperlink ref="W34" r:id="rId63"/>
+    <hyperlink ref="Y30" r:id="rId64"/>
+    <hyperlink ref="W30" r:id="rId65"/>
+    <hyperlink ref="X30" r:id="rId66"/>
+    <hyperlink ref="W20" r:id="rId67"/>
+    <hyperlink ref="W10" r:id="rId68"/>
+    <hyperlink ref="X10" r:id="rId69"/>
     <hyperlink ref="I35" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>